<commit_message>
modify load_file_receipt, fix repeat load
</commit_message>
<xml_diff>
--- a/warehouseDRF/ACCOUNTING/xls/receipt.xlsx
+++ b/warehouseDRF/ACCOUNTING/xls/receipt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">товар</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">крикрос</t>
+  </si>
+  <si>
+    <t xml:space="preserve">крестнакрест</t>
   </si>
 </sst>
 </file>
@@ -278,10 +281,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -319,7 +322,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,6 +349,14 @@
         <v>666</v>
       </c>
       <c r="C7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>